<commit_message>
Add tvs to 303
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-303-BOM-JLC.xlsx
+++ b/Manufacturing Files/bitaxeHex-303-BOM-JLC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="259">
   <si>
     <t>Designator</t>
   </si>
@@ -795,6 +795,15 @@
   </si>
   <si>
     <t>BM1366_mode0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C26174720</t>
+  </si>
+  <si>
+    <t>DFN1610-2L</t>
   </si>
 </sst>
 </file>
@@ -1665,10 +1674,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2701,6 +2710,20 @@
         <v>243</v>
       </c>
     </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B63" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" t="s">
+        <v>258</v>
+      </c>
+      <c r="D63">
+        <v>824045812</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>